<commit_message>
changes so no rats sniff less than 0 times
</commit_message>
<xml_diff>
--- a/conference_2_take_2_dataset.xlsx
+++ b/conference_2_take_2_dataset.xlsx
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>83.2516456455854</v>
+        <v>74.64459191154116</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>27.26454974434564</v>
+        <v>53.53193131047207</v>
       </c>
     </row>
     <row r="3">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>86.59232262544485</v>
+        <v>77.79957736918256</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>15.21348567409279</v>
+        <v>44.1962202884235</v>
       </c>
     </row>
     <row r="4">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>78.49252436513436</v>
+        <v>68.25747707927708</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>35.9183004518616</v>
+        <v>43.90897538890447</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>63.37244171348113</v>
+        <v>62.567507910511</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>23.84343687389897</v>
+        <v>43.82062369509142</v>
       </c>
     </row>
     <row r="6">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>77.56191933637528</v>
+        <v>79.45479774349043</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>46.06927608643068</v>
+        <v>45.99593198831673</v>
       </c>
     </row>
     <row r="7">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>76.36715347874446</v>
+        <v>72.89066212829194</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>28.32616205525566</v>
+        <v>56.50550174673216</v>
       </c>
     </row>
     <row r="8">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>82.24012013648392</v>
+        <v>83.67919229603444</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>34.3695012459461</v>
+        <v>29.36094269240385</v>
       </c>
     </row>
     <row r="9">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>62.38723060292441</v>
+        <v>80.3622518992558</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>38.50823486454264</v>
+        <v>38.24099094636163</v>
       </c>
     </row>
     <row r="10">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>85.66001550949495</v>
+        <v>76.11431442617257</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>34.65488052352694</v>
+        <v>42.98769925446699</v>
       </c>
     </row>
     <row r="11">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>86.73412361721242</v>
+        <v>64.86810736746972</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>51.81974669466162</v>
+        <v>30.65629709984288</v>
       </c>
     </row>
     <row r="12">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>93.99451854836494</v>
+        <v>83.54070581805159</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>33.39879091261498</v>
+        <v>44.64090637714941</v>
       </c>
     </row>
     <row r="13">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>72.3161054937042</v>
+        <v>69.3016451409988</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>29.61188487784658</v>
+        <v>39.79535297528177</v>
       </c>
     </row>
     <row r="14">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>62.85906044187232</v>
+        <v>64.07067292424753</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>59.31076466254918</v>
+        <v>35.10688021324463</v>
       </c>
     </row>
     <row r="15">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>66.81690945392602</v>
+        <v>58.63634663365594</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>34.3950523177832</v>
+        <v>27.37920026927899</v>
       </c>
     </row>
     <row r="16">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>62.30285021347979</v>
+        <v>79.90233306284325</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>47.13607321270675</v>
+        <v>35.31865926703776</v>
       </c>
     </row>
     <row r="17">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>83.85581734642585</v>
+        <v>78.68947835840788</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>18.52516519892289</v>
+        <v>25.05951971248025</v>
       </c>
     </row>
     <row r="18">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>78.71065366968244</v>
+        <v>67.63883763127679</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>30.02360899435697</v>
+        <v>28.04653147469527</v>
       </c>
     </row>
     <row r="19">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>65.46899153896902</v>
+        <v>78.00613789439682</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>21.48309877370929</v>
+        <v>40.62617253837106</v>
       </c>
     </row>
     <row r="20">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>72.19537272418282</v>
+        <v>71.32647941919515</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>21.85298142840819</v>
+        <v>49.02854796949428</v>
       </c>
     </row>
     <row r="21">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>72.4615537860908</v>
+        <v>55.67445537681422</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>37.06488173454017</v>
+        <v>66.34043318232831</v>
       </c>
     </row>
     <row r="22">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>70.64719664327238</v>
+        <v>77.13857069733808</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>26.51194878443284</v>
+        <v>44.92367644819461</v>
       </c>
     </row>
     <row r="23">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>82.7756451425122</v>
+        <v>85.45290846315524</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>28.4432020580313</v>
+        <v>39.92114576591907</v>
       </c>
     </row>
     <row r="24">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>71.26754595681099</v>
+        <v>84.95626234511286</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>48.02168493749296</v>
+        <v>33.69302428015901</v>
       </c>
     </row>
     <row r="25">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>65.99496849512045</v>
+        <v>59.00844282997936</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>32.4059421506056</v>
+        <v>52.54439988642599</v>
       </c>
     </row>
     <row r="26">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>68.1286031717913</v>
+        <v>70.76234776841625</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>46.5111706843764</v>
+        <v>41.52265164190553</v>
       </c>
     </row>
   </sheetData>
@@ -854,13 +854,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7635.714824202161</v>
+        <v>7948.948993232589</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>7583.428466389224</v>
+        <v>7330.044034729261</v>
       </c>
     </row>
     <row r="3">
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7402.910705640867</v>
+        <v>7403.740298930814</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7943.791229169782</v>
+        <v>7551.25027202397</v>
       </c>
     </row>
     <row r="4">
@@ -882,13 +882,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7551.866690333967</v>
+        <v>7669.789842812178</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>7924.010556275418</v>
+        <v>7949.08707901059</v>
       </c>
     </row>
     <row r="5">
@@ -896,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>7254.11797175339</v>
+        <v>7304.023900438465</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>7957.256041989574</v>
+        <v>7660.139678677036</v>
       </c>
     </row>
     <row r="6">
@@ -910,13 +910,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7696.152526945392</v>
+        <v>7124.413447880956</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>7718.985552003414</v>
+        <v>7353.638296474589</v>
       </c>
     </row>
     <row r="7">
@@ -924,13 +924,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>7905.487792567634</v>
+        <v>7824.888132293884</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>7485.677467715894</v>
+        <v>7297.2460705418</v>
       </c>
     </row>
     <row r="8">
@@ -938,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7738.926160184736</v>
+        <v>7376.074420799814</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7034.11586648588</v>
+        <v>7795.23332365447</v>
       </c>
     </row>
     <row r="9">
@@ -952,13 +952,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>7656.250253469144</v>
+        <v>7839.163694628411</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>7532.00557549179</v>
+        <v>7968.757425537809</v>
       </c>
     </row>
     <row r="10">
@@ -966,13 +966,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7445.39520519035</v>
+        <v>7271.390100263529</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>7678.019071865774</v>
+        <v>7959.323473740525</v>
       </c>
     </row>
     <row r="11">
@@ -980,13 +980,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>7176.076589706288</v>
+        <v>7712.956091610922</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>7749.496630517954</v>
+        <v>7446.657228425614</v>
       </c>
     </row>
     <row r="12">
@@ -994,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>7308.882146399756</v>
+        <v>7782.189628751286</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>7667.396891320777</v>
+        <v>7913.327202069988</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>7886.33728617666</v>
+        <v>7693.010954805378</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>7789.141490031271</v>
+        <v>7930.39267607786</v>
       </c>
     </row>
     <row r="14">
@@ -1022,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>7881.41993867154</v>
+        <v>7799.388542890402</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>7684.625476239435</v>
+        <v>7663.027033557164</v>
       </c>
     </row>
     <row r="15">
@@ -1036,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>6577.891161851743</v>
+        <v>7796.731691450375</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>7884.079831114909</v>
+        <v>7385.574541402624</v>
       </c>
     </row>
     <row r="16">
@@ -1050,13 +1050,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>7880.165201293026</v>
+        <v>7560.54445385029</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>7654.384539363201</v>
+        <v>7858.768700427429</v>
       </c>
     </row>
     <row r="17">
@@ -1064,13 +1064,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>7295.553978296226</v>
+        <v>7252.506255459401</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>7714.001241972629</v>
+        <v>6844.482253735398</v>
       </c>
     </row>
     <row r="18">
@@ -1078,13 +1078,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>7527.151329380358</v>
+        <v>7854.120613743521</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>7743.614083004461</v>
+        <v>7253.165491776032</v>
       </c>
     </row>
     <row r="19">
@@ -1092,13 +1092,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>7747.400727483573</v>
+        <v>7891.530369964452</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>7847.024573855455</v>
+        <v>7818.923871337322</v>
       </c>
     </row>
     <row r="20">
@@ -1106,13 +1106,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>7860.795543939253</v>
+        <v>7204.307032627624</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>7557.291690373006</v>
+        <v>7460.77318026198</v>
       </c>
     </row>
     <row r="21">
@@ -1120,13 +1120,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>7734.386960427209</v>
+        <v>7881.368860978941</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>7453.251823809669</v>
+        <v>7270.508754624054</v>
       </c>
     </row>
   </sheetData>
@@ -1175,13 +1175,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8410566645127046</v>
+        <v>0.8224587558286037</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5982555499346431</v>
+        <v>0.5027662074338511</v>
       </c>
     </row>
     <row r="3">
@@ -1189,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8253786795255998</v>
+        <v>0.836858309259234</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5222594021649209</v>
+        <v>0.5292633276738207</v>
       </c>
     </row>
     <row r="4">
@@ -1203,13 +1203,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8120686041860132</v>
+        <v>0.803863577143574</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5989928549952143</v>
+        <v>0.5966788849439597</v>
       </c>
     </row>
     <row r="5">
@@ -1217,13 +1217,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8359921242433008</v>
+        <v>0.8995882286228075</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5197625452336839</v>
+        <v>0.5752164298769785</v>
       </c>
     </row>
     <row r="6">
@@ -1231,13 +1231,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8447232671136817</v>
+        <v>0.8716722430876214</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5774676664020275</v>
+        <v>0.5277817741474468</v>
       </c>
     </row>
     <row r="7">
@@ -1245,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8298542986401937</v>
+        <v>0.8538810163113871</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5018005448005656</v>
+        <v>0.5604364232894699</v>
       </c>
     </row>
     <row r="8">
@@ -1259,13 +1259,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8062969156784833</v>
+        <v>0.8972858291232749</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5121481634514358</v>
+        <v>0.567622256955749</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1273,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8064511269951508</v>
+        <v>0.8811329475520486</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5107108112053942</v>
+        <v>0.5805618560556793</v>
       </c>
     </row>
     <row r="10">
@@ -1287,13 +1287,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.811900506623345</v>
+        <v>0.8281076979462416</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5921393347584329</v>
+        <v>0.5776364007085217</v>
       </c>
     </row>
     <row r="11">
@@ -1301,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8338574333981886</v>
+        <v>0.8588516546661956</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5572509993838869</v>
+        <v>0.5286015205874899</v>
       </c>
     </row>
     <row r="12">
@@ -1315,13 +1315,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8700970112089786</v>
+        <v>0.8631638976657395</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5050532070365754</v>
+        <v>0.5122858323459869</v>
       </c>
     </row>
     <row r="13">
@@ -1329,13 +1329,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8955157364351714</v>
+        <v>0.8945252682833955</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5026361257713503</v>
+        <v>0.5952884186042857</v>
       </c>
     </row>
     <row r="14">
@@ -1343,13 +1343,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8435642783844814</v>
+        <v>0.877976478931229</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5136936997021412</v>
+        <v>0.5477127387060678</v>
       </c>
     </row>
     <row r="15">
@@ -1357,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8434200206256752</v>
+        <v>0.8214303429523636</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5085334359972433</v>
+        <v>0.5556391684518823</v>
       </c>
     </row>
     <row r="16">
@@ -1371,13 +1371,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8539780041707196</v>
+        <v>0.8241936837540611</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5713738215656593</v>
+        <v>0.5586109261312991</v>
       </c>
     </row>
     <row r="17">
@@ -1385,13 +1385,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.8418587161200594</v>
+        <v>0.8390866825174598</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5665753695309546</v>
+        <v>0.5282127405820245</v>
       </c>
     </row>
     <row r="18">
@@ -1399,13 +1399,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.831694535670139</v>
+        <v>0.8938476687425383</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5408030684848573</v>
+        <v>0.5280427052499826</v>
       </c>
     </row>
     <row r="19">
@@ -1413,13 +1413,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8603023687319428</v>
+        <v>0.8121574965468277</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5595505039156432</v>
+        <v>0.5933528444430032</v>
       </c>
     </row>
     <row r="20">
@@ -1427,13 +1427,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8840345624290976</v>
+        <v>0.8671055791957805</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5475520544791694</v>
+        <v>0.5826606850220952</v>
       </c>
     </row>
     <row r="21">
@@ -1441,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8190054292169692</v>
+        <v>0.8111441111755445</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5948305272990309</v>
+        <v>0.5280222615754893</v>
       </c>
     </row>
     <row r="22">
@@ -1455,13 +1455,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.816411578452673</v>
+        <v>0.8460237204777739</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5138319853351031</v>
+        <v>0.5569959111976449</v>
       </c>
     </row>
     <row r="23">
@@ -1469,13 +1469,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8897427919357002</v>
+        <v>0.8494315723746306</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5849180590094614</v>
+        <v>0.5086757551311737</v>
       </c>
     </row>
     <row r="24">
@@ -1483,13 +1483,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8910111623348717</v>
+        <v>0.8718219629307009</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5083607523087955</v>
+        <v>0.5834639627499791</v>
       </c>
     </row>
     <row r="25">
@@ -1497,13 +1497,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.8227606846835344</v>
+        <v>0.8179249107346159</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5469716467629158</v>
+        <v>0.5430561825925871</v>
       </c>
     </row>
     <row r="26">
@@ -1511,13 +1511,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8095271627287712</v>
+        <v>0.8094218960940464</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5570949085282898</v>
+        <v>0.5390369922908674</v>
       </c>
     </row>
     <row r="27">
@@ -1525,13 +1525,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8555016428382913</v>
+        <v>0.8619442238021385</v>
       </c>
       <c r="C27" t="n">
         <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5263346662595717</v>
+        <v>0.5296667707524569</v>
       </c>
     </row>
     <row r="28">
@@ -1539,13 +1539,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.845410385537031</v>
+        <v>0.8402235028409004</v>
       </c>
       <c r="C28" t="n">
         <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5806950588562583</v>
+        <v>0.5847831289948553</v>
       </c>
     </row>
     <row r="29">
@@ -1553,13 +1553,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8027480069803621</v>
+        <v>0.8380869478811868</v>
       </c>
       <c r="C29" t="n">
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5201559253617722</v>
+        <v>0.577456471689147</v>
       </c>
     </row>
     <row r="30">
@@ -1567,13 +1567,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.874735706521641</v>
+        <v>0.8388029948023309</v>
       </c>
       <c r="C30" t="n">
         <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>0.521245714789289</v>
+        <v>0.5242557242203325</v>
       </c>
     </row>
     <row r="31">
@@ -1581,13 +1581,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.867444370829531</v>
+        <v>0.8600348142253528</v>
       </c>
       <c r="C31" t="n">
         <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5793477517758834</v>
+        <v>0.5163501443111291</v>
       </c>
     </row>
     <row r="32">
@@ -1595,13 +1595,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8054434767179388</v>
+        <v>0.8002868770387285</v>
       </c>
       <c r="C32" t="n">
         <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5427510744816932</v>
+        <v>0.5552022616367698</v>
       </c>
     </row>
     <row r="33">
@@ -1609,13 +1609,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8240826942580046</v>
+        <v>0.8939124443867561</v>
       </c>
       <c r="C33" t="n">
         <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5010627547468168</v>
+        <v>0.5705763462411173</v>
       </c>
     </row>
     <row r="34">
@@ -1623,13 +1623,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.8064538515851518</v>
+        <v>0.8072141915681725</v>
       </c>
       <c r="C34" t="n">
         <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5609298010681504</v>
+        <v>0.5675684172003516</v>
       </c>
     </row>
     <row r="35">
@@ -1637,13 +1637,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.8616813303466885</v>
+        <v>0.8664670061428433</v>
       </c>
       <c r="C35" t="n">
         <v>34</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5973839775033885</v>
+        <v>0.520251884015163</v>
       </c>
     </row>
     <row r="36">
@@ -1651,13 +1651,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.8136839730331802</v>
+        <v>0.8196337716482129</v>
       </c>
       <c r="C36" t="n">
         <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5641973429320974</v>
+        <v>0.5590384367318701</v>
       </c>
     </row>
     <row r="37">
@@ -1665,13 +1665,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8840160298638565</v>
+        <v>0.8632985349006363</v>
       </c>
       <c r="C37" t="n">
         <v>36</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5867807154314736</v>
+        <v>0.5896279514705077</v>
       </c>
     </row>
     <row r="38">
@@ -1679,13 +1679,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.8853715899321457</v>
+        <v>0.8575206429039534</v>
       </c>
       <c r="C38" t="n">
         <v>37</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5031902830310518</v>
+        <v>0.561709539934715</v>
       </c>
     </row>
     <row r="39">
@@ -1693,13 +1693,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.8170904140594502</v>
+        <v>0.8731667691523783</v>
       </c>
       <c r="C39" t="n">
         <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5061420350787004</v>
+        <v>0.5275160213069343</v>
       </c>
     </row>
     <row r="40">
@@ -1707,13 +1707,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.8290063854632551</v>
+        <v>0.8551695575572501</v>
       </c>
       <c r="C40" t="n">
         <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5573277102076675</v>
+        <v>0.5466327026636751</v>
       </c>
     </row>
     <row r="41">
@@ -1721,13 +1721,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.8701593990176842</v>
+        <v>0.8835610427801582</v>
       </c>
       <c r="C41" t="n">
         <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5398535830146878</v>
+        <v>0.5817698109560243</v>
       </c>
     </row>
   </sheetData>
@@ -1776,13 +1776,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -1790,13 +1790,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -1810,7 +1810,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -1818,13 +1818,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -1832,13 +1832,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -1846,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -1874,13 +1874,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -1888,13 +1888,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1902,13 +1902,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -1916,13 +1916,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -1936,7 +1936,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -1944,13 +1944,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
@@ -1964,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -1972,13 +1972,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
@@ -1986,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
@@ -2000,13 +2000,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -2014,13 +2014,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
@@ -2028,13 +2028,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
@@ -2042,7 +2042,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>-0</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
@@ -2056,13 +2056,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>-2</v>
+        <v>-0</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -2070,13 +2070,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>-0</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
@@ -2090,7 +2090,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
@@ -2098,13 +2098,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>-0</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
@@ -2112,7 +2112,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>-0</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>

</xml_diff>